<commit_message>
Added ex marire updates
</commit_message>
<xml_diff>
--- a/Teaching/2017-2018/Stat web page/results/Tabel_Statistica_feb_17_2018.xlsx
+++ b/Teaching/2017-2018/Stat web page/results/Tabel_Statistica_feb_17_2018.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amari\OneDrive\Teaching\Curs Universitate Eu\2017 - 2018\Statistica\rezultate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amari\OneDrive\GitHub\AlexAmarioarei.github.io\Teaching\2017-2018\Stat web page\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="213" documentId="8_{7079A115-55D5-491C-8336-ADE05FBC62F7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{26082C5F-F281-4792-9DB0-31BFDC847E8B}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="8_{7079A115-55D5-491C-8336-ADE05FBC62F7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{7F1A349D-9144-46A5-AB2A-ED9980962A16}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13808" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabel_Statistica!$A$1:$J$82</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -995,14 +995,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1337,7 +1330,7 @@
   <dimension ref="A1:O82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O56" sqref="O56"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5286,17 +5279,17 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="L2">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
       <formula>4.01</formula>
       <formula>4.4999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>4.01</formula>
       <formula>4.4999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>5.1</formula>
       <formula>5.4999</formula>
     </cfRule>

</xml_diff>